<commit_message>
Fix: Strict date filtering. Removed +/- 1 day buffer to prevent history pollution in Home.
</commit_message>
<xml_diff>
--- a/backend/plantilla_planificacion_v2.xlsx
+++ b/backend/plantilla_planificacion_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd171dda8de17894/Desktop/cerebro-patio/Cerebro/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_2BB1D69C5BC0D3126FBB2C115931B0B165A5FE2E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8A9A613-D306-4E6F-BF97-B98D77D47446}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="11_2BB1D69C5BC0D3126FBB2C115931B0B165A5FE2E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17D7E8E1-1493-49D5-99AD-CC2BFD578EF6}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="2500" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -79,16 +79,16 @@
     <t>Pedro Pascal</t>
   </si>
   <si>
-    <t>HCCR34</t>
-  </si>
-  <si>
-    <t>BSBJ92</t>
-  </si>
-  <si>
-    <t>YALA</t>
-  </si>
-  <si>
-    <t>VALU</t>
+    <t>BRINKS</t>
+  </si>
+  <si>
+    <t>SOPROLE</t>
+  </si>
+  <si>
+    <t>BSBJ90</t>
+  </si>
+  <si>
+    <t>HCCR30</t>
   </si>
 </sst>
 </file>
@@ -454,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -510,10 +510,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
-        <v>46018</v>
+        <v>46019</v>
       </c>
       <c r="B2">
-        <v>413345</v>
+        <v>4133457</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -537,18 +537,18 @@
         <v>17</v>
       </c>
       <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
         <v>19</v>
-      </c>
-      <c r="K2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
-        <v>46018</v>
+        <v>46019</v>
       </c>
       <c r="B3">
-        <v>413235</v>
+        <v>4132357</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -572,10 +572,10 @@
         <v>18</v>
       </c>
       <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
         <v>20</v>
-      </c>
-      <c r="K3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Fix: Home defaults to Latest Plan (Max Date) instead of Today
</commit_message>
<xml_diff>
--- a/backend/plantilla_planificacion_v2.xlsx
+++ b/backend/plantilla_planificacion_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd171dda8de17894/Desktop/cerebro-patio/Cerebro/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="11_2BB1D69C5BC0D3126FBB2C115931B0B165A5FE2E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17D7E8E1-1493-49D5-99AD-CC2BFD578EF6}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="11_2BB1D69C5BC0D3126FBB2C115931B0B165A5FE2E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{851FF36F-2930-4C47-93CF-F250B753321E}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,16 +79,16 @@
     <t>Pedro Pascal</t>
   </si>
   <si>
-    <t>BRINKS</t>
-  </si>
-  <si>
-    <t>SOPROLE</t>
-  </si>
-  <si>
-    <t>BSBJ90</t>
-  </si>
-  <si>
-    <t>HCCR30</t>
+    <t>ECOTRANS</t>
+  </si>
+  <si>
+    <t>AGRETRANS</t>
+  </si>
+  <si>
+    <t>BSBJ91</t>
+  </si>
+  <si>
+    <t>HCCR31</t>
   </si>
 </sst>
 </file>
@@ -454,14 +454,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.73046875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.9296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.06640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.19921875" bestFit="1" customWidth="1"/>
@@ -510,10 +510,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
-        <v>46019</v>
+        <v>46020</v>
       </c>
       <c r="B2">
-        <v>4133457</v>
+        <v>413345733</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -545,10 +545,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
-        <v>46019</v>
+        <v>46020</v>
       </c>
       <c r="B3">
-        <v>4132357</v>
+        <v>413235733</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Fix: Signature now registers for specific Plan Date, not Upload Date.
</commit_message>
<xml_diff>
--- a/backend/plantilla_planificacion_v2.xlsx
+++ b/backend/plantilla_planificacion_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd171dda8de17894/Desktop/cerebro-patio/Cerebro/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="11_2BB1D69C5BC0D3126FBB2C115931B0B165A5FE2E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{851FF36F-2930-4C47-93CF-F250B753321E}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="11_2BB1D69C5BC0D3126FBB2C115931B0B165A5FE2E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAFDE392-26F7-40A1-AC36-24EA0A184C70}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,16 +79,16 @@
     <t>Pedro Pascal</t>
   </si>
   <si>
-    <t>ECOTRANS</t>
-  </si>
-  <si>
-    <t>AGRETRANS</t>
-  </si>
-  <si>
     <t>BSBJ91</t>
   </si>
   <si>
     <t>HCCR31</t>
+  </si>
+  <si>
+    <t>HOLA</t>
+  </si>
+  <si>
+    <t>CHAO</t>
   </si>
 </sst>
 </file>
@@ -455,7 +455,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -510,10 +510,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
-        <v>46020</v>
+        <v>46021</v>
       </c>
       <c r="B2">
-        <v>413345733</v>
+        <v>413345734</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -537,18 +537,18 @@
         <v>17</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
-        <v>46020</v>
+        <v>46021</v>
       </c>
       <c r="B3">
-        <v>413235733</v>
+        <v>413235734</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -572,10 +572,10 @@
         <v>18</v>
       </c>
       <c r="J3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Milestone: MVP Core Flow Complete. History, Smart Home, and Strict Signatures.
</commit_message>
<xml_diff>
--- a/backend/plantilla_planificacion_v2.xlsx
+++ b/backend/plantilla_planificacion_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd171dda8de17894/Desktop/cerebro-patio/Cerebro/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="11_2BB1D69C5BC0D3126FBB2C115931B0B165A5FE2E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAFDE392-26F7-40A1-AC36-24EA0A184C70}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="11_2BB1D69C5BC0D3126FBB2C115931B0B165A5FE2E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97E1FBB6-9306-4208-A902-413ED423E22E}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,10 +85,10 @@
     <t>HCCR31</t>
   </si>
   <si>
-    <t>HOLA</t>
-  </si>
-  <si>
-    <t>CHAO</t>
+    <t>NANO</t>
+  </si>
+  <si>
+    <t>CHRIS</t>
   </si>
 </sst>
 </file>
@@ -454,14 +454,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.73046875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.9296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.06640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.19921875" bestFit="1" customWidth="1"/>
@@ -510,10 +510,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B2">
-        <v>413345734</v>
+        <v>4133457345</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -545,10 +545,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B3">
-        <v>413235734</v>
+        <v>4132357345</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Fix planning email, restore professional template, improve task deduplication
</commit_message>
<xml_diff>
--- a/backend/plantilla_planificacion_v2.xlsx
+++ b/backend/plantilla_planificacion_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd171dda8de17894/Desktop/cerebro-patio/Cerebro/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="11_2BB1D69C5BC0D3126FBB2C115931B0B165A5FE2E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97E1FBB6-9306-4208-A902-413ED423E22E}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="11_2BB1D69C5BB0582E3B7825115931B0B165A5FE2E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF9FAF09-429A-42F4-9A51-A42CB476D185}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
   <si>
     <t>fecha</t>
   </si>
@@ -73,22 +73,73 @@
     <t>Región Metropolitana de Santiago.</t>
   </si>
   <si>
+    <t>HCCR38</t>
+  </si>
+  <si>
+    <t>CIAL_ALIMENTOS</t>
+  </si>
+  <si>
+    <t>BSBJ91</t>
+  </si>
+  <si>
+    <t>inmediata</t>
+  </si>
+  <si>
+    <t>Soporte</t>
+  </si>
+  <si>
+    <t>Botón Alámbrico Tablero</t>
+  </si>
+  <si>
+    <t>RODRIGO DE ARAYA 2821, MACUL</t>
+  </si>
+  <si>
+    <t>MACUL</t>
+  </si>
+  <si>
+    <t>VDVP13</t>
+  </si>
+  <si>
+    <t>COMERCIAL_DIBOR</t>
+  </si>
+  <si>
+    <t>alta</t>
+  </si>
+  <si>
+    <t>MDVR 4ch sin IA</t>
+  </si>
+  <si>
+    <t>EL VENTISQUERO 1250, RENCA</t>
+  </si>
+  <si>
+    <t>RENCA</t>
+  </si>
+  <si>
+    <t>KHSJ34</t>
+  </si>
+  <si>
+    <t>SOPROLE</t>
+  </si>
+  <si>
+    <t>AV. LO ESPEJO 1300, MAIPU</t>
+  </si>
+  <si>
+    <t>MAIPU</t>
+  </si>
+  <si>
+    <t>GENERADOR_SANTIAGO_19</t>
+  </si>
+  <si>
+    <t>LUREYE</t>
+  </si>
+  <si>
+    <t>GENERADOR_SANTIAGO_18</t>
+  </si>
+  <si>
     <t>Juan Perez</t>
   </si>
   <si>
     <t>Pedro Pascal</t>
-  </si>
-  <si>
-    <t>BSBJ91</t>
-  </si>
-  <si>
-    <t>HCCR31</t>
-  </si>
-  <si>
-    <t>NANO</t>
-  </si>
-  <si>
-    <t>CHRIS</t>
   </si>
 </sst>
 </file>
@@ -454,23 +505,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.9296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.06640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.19921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.1328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.1328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.73046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.53125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.53125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.06640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
@@ -510,10 +561,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
-        <v>46022</v>
+        <v>46011</v>
       </c>
       <c r="B2">
-        <v>4133457345</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -534,21 +585,21 @@
         <v>16</v>
       </c>
       <c r="I2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" t="s">
-        <v>20</v>
-      </c>
       <c r="K2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
-        <v>46022</v>
+        <v>46011</v>
       </c>
       <c r="B3">
-        <v>4132357345</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -569,26 +620,154 @@
         <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="J3" t="s">
         <v>19</v>
       </c>
       <c r="K3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2">
+        <v>46011</v>
+      </c>
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2">
+        <v>46011</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A6" s="2"/>
+      <c r="A6" s="2">
+        <v>46011</v>
+      </c>
+      <c r="B6">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A7" s="2"/>
+      <c r="A7" s="2">
+        <v>46011</v>
+      </c>
+      <c r="B7">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fix import errors in finance and sheets service causing boot crash
</commit_message>
<xml_diff>
--- a/backend/plantilla_planificacion_v2.xlsx
+++ b/backend/plantilla_planificacion_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd171dda8de17894/Desktop/cerebro-patio/Cerebro/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="11_2BB1D69C5BB0582E3B7825115931B0B165A5FE2E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF9FAF09-429A-42F4-9A51-A42CB476D185}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="11_2BB1D69C5BB0582E3B7825115931B0B165A5FE2E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4C00128-A731-40B4-A797-9D65FC850080}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -506,7 +506,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -561,10 +561,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
-        <v>46011</v>
+        <v>46020</v>
       </c>
       <c r="B2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -596,10 +596,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
-        <v>46011</v>
+        <v>46020</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -631,10 +631,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
-        <v>46011</v>
+        <v>46020</v>
       </c>
       <c r="B4">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -666,10 +666,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
-        <v>46011</v>
+        <v>46020</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>27</v>
@@ -701,10 +701,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
-        <v>46011</v>
+        <v>46020</v>
       </c>
       <c r="B6">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -736,10 +736,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
-        <v>46011</v>
+        <v>46020</v>
       </c>
       <c r="B7">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Fix SQLAlchemy relationship mapping error for User.expenses
</commit_message>
<xml_diff>
--- a/backend/plantilla_planificacion_v2.xlsx
+++ b/backend/plantilla_planificacion_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd171dda8de17894/Desktop/cerebro-patio/Cerebro/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="11_2BB1D69C5BB0582E3B7825115931B0B165A5FE2E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4C00128-A731-40B4-A797-9D65FC850080}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="11_2BB1D69C5BB0582E3B7825115931B0B165A5FE2E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C34CC87F-0815-49CD-95DA-73859E9B4B3B}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -216,6 +216,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -506,7 +510,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -564,7 +568,7 @@
         <v>46020</v>
       </c>
       <c r="B2">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -599,7 +603,7 @@
         <v>46020</v>
       </c>
       <c r="B3">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -634,7 +638,7 @@
         <v>46020</v>
       </c>
       <c r="B4">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -669,7 +673,7 @@
         <v>46020</v>
       </c>
       <c r="B5">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
         <v>27</v>
@@ -704,7 +708,7 @@
         <v>46020</v>
       </c>
       <c r="B6">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -739,7 +743,7 @@
         <v>46020</v>
       </c>
       <c r="B7">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Upgrade Workday Closing Email to Professional Template
</commit_message>
<xml_diff>
--- a/backend/plantilla_planificacion_v2.xlsx
+++ b/backend/plantilla_planificacion_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd171dda8de17894/Desktop/cerebro-patio/Cerebro/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="11_2BB1D69C5BB0582E3B7825115931B0B165A5FE2E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C34CC87F-0815-49CD-95DA-73859E9B4B3B}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="11_2BB1D69C5B505F711B583E11592FA0B55413FAA7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{786DB716-75FB-49EE-BA91-7A4046E7FF40}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>fecha</t>
   </si>
@@ -55,91 +55,58 @@
     <t>cliente</t>
   </si>
   <si>
+    <t>urgente</t>
+  </si>
+  <si>
+    <t>Soporte</t>
+  </si>
+  <si>
+    <t>Antena GPS, Corta Corriente Remoto</t>
+  </si>
+  <si>
+    <t>AMERICO VESPUCIO NORTE 2341, PUDAHUEL</t>
+  </si>
+  <si>
+    <t>PUDAHUEL</t>
+  </si>
+  <si>
+    <t>Región Metropolitana de Santiago.</t>
+  </si>
+  <si>
+    <t>PRSV10</t>
+  </si>
+  <si>
+    <t>CIAL_ALIMENTOS</t>
+  </si>
+  <si>
+    <t>Antena GPS</t>
+  </si>
+  <si>
+    <t>VE041-LCSH40</t>
+  </si>
+  <si>
     <t>normal</t>
   </si>
   <si>
-    <t>Instalación</t>
-  </si>
-  <si>
-    <t>Antena GPS</t>
-  </si>
-  <si>
-    <t>AMERICO VESPUCIO 2341 PUDAHUEL</t>
-  </si>
-  <si>
-    <t>PUDAHUEL</t>
-  </si>
-  <si>
-    <t>Región Metropolitana de Santiago.</t>
-  </si>
-  <si>
-    <t>HCCR38</t>
-  </si>
-  <si>
-    <t>CIAL_ALIMENTOS</t>
-  </si>
-  <si>
-    <t>BSBJ91</t>
-  </si>
-  <si>
-    <t>inmediata</t>
-  </si>
-  <si>
-    <t>Soporte</t>
-  </si>
-  <si>
-    <t>Botón Alámbrico Tablero</t>
-  </si>
-  <si>
-    <t>RODRIGO DE ARAYA 2821, MACUL</t>
-  </si>
-  <si>
-    <t>MACUL</t>
-  </si>
-  <si>
-    <t>VDVP13</t>
-  </si>
-  <si>
-    <t>COMERCIAL_DIBOR</t>
-  </si>
-  <si>
-    <t>alta</t>
-  </si>
-  <si>
-    <t>MDVR 4ch sin IA</t>
-  </si>
-  <si>
-    <t>EL VENTISQUERO 1250, RENCA</t>
-  </si>
-  <si>
-    <t>RENCA</t>
-  </si>
-  <si>
-    <t>KHSJ34</t>
+    <t>VCVF53</t>
+  </si>
+  <si>
+    <t>HPWV83</t>
+  </si>
+  <si>
+    <t>Juan Parez</t>
+  </si>
+  <si>
+    <t>Pedro Pascal</t>
   </si>
   <si>
     <t>SOPROLE</t>
   </si>
   <si>
-    <t>AV. LO ESPEJO 1300, MAIPU</t>
-  </si>
-  <si>
-    <t>MAIPU</t>
-  </si>
-  <si>
-    <t>GENERADOR_SANTIAGO_19</t>
-  </si>
-  <si>
-    <t>LUREYE</t>
-  </si>
-  <si>
-    <t>GENERADOR_SANTIAGO_18</t>
-  </si>
-  <si>
-    <t>Juan Perez</t>
-  </si>
-  <si>
-    <t>Pedro Pascal</t>
+    <t>AGUNSA</t>
+  </si>
+  <si>
+    <t>BRINKS</t>
   </si>
 </sst>
 </file>
@@ -200,7 +167,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -216,10 +183,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -507,25 +470,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.9296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.59765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.53125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.06640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.53125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.06640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
@@ -568,7 +531,7 @@
         <v>46020</v>
       </c>
       <c r="B2">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -589,7 +552,7 @@
         <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="J2" t="s">
         <v>17</v>
@@ -603,7 +566,7 @@
         <v>46020</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -612,7 +575,7 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
@@ -624,13 +587,13 @@
         <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="J3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
@@ -638,34 +601,31 @@
         <v>46020</v>
       </c>
       <c r="B4">
+        <v>102</v>
+      </c>
+      <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
       <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H4" t="s">
         <v>16</v>
       </c>
       <c r="I4" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="J4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
@@ -673,104 +633,31 @@
         <v>46020</v>
       </c>
       <c r="B5">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H5" t="s">
         <v>16</v>
       </c>
       <c r="I5" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="J5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="K5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A6" s="2">
-        <v>46020</v>
-      </c>
-      <c r="B6">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A7" s="2">
-        <v>46020</v>
-      </c>
-      <c r="B7">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J7" t="s">
-        <v>37</v>
-      </c>
-      <c r="K7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HOTFIX: Use BackgroundTasks for Workday Email to prevent 502 Timeouts
</commit_message>
<xml_diff>
--- a/backend/plantilla_planificacion_v2.xlsx
+++ b/backend/plantilla_planificacion_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd171dda8de17894/Desktop/cerebro-patio/Cerebro/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_2BB1D69C5B505F711B583E11592FA0B55413FAA7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{786DB716-75FB-49EE-BA91-7A4046E7FF40}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_2BB1D69C5B505F711B583E11592FA0B55413FAA7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB8548F3-A11A-4D31-B285-571A22BCE96E}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>fecha</t>
   </si>
@@ -76,37 +76,10 @@
     <t>PRSV10</t>
   </si>
   <si>
-    <t>CIAL_ALIMENTOS</t>
-  </si>
-  <si>
-    <t>Antena GPS</t>
-  </si>
-  <si>
-    <t>VE041-LCSH40</t>
-  </si>
-  <si>
-    <t>normal</t>
-  </si>
-  <si>
-    <t>VCVF53</t>
-  </si>
-  <si>
-    <t>HPWV83</t>
-  </si>
-  <si>
-    <t>Juan Parez</t>
-  </si>
-  <si>
-    <t>Pedro Pascal</t>
-  </si>
-  <si>
-    <t>SOPROLE</t>
-  </si>
-  <si>
-    <t>AGUNSA</t>
-  </si>
-  <si>
-    <t>BRINKS</t>
+    <t>Juan Perez</t>
+  </si>
+  <si>
+    <t>HOLA prueba</t>
   </si>
 </sst>
 </file>
@@ -183,6 +156,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -470,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -552,112 +529,13 @@
         <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="J2" t="s">
         <v>17</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A3" s="2">
-        <v>46020</v>
-      </c>
-      <c r="B3">
-        <v>101</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
         <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A4" s="2">
-        <v>46020</v>
-      </c>
-      <c r="B4">
-        <v>102</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A5" s="2">
-        <v>46020</v>
-      </c>
-      <c r="B5">
-        <v>103</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FEATURE: Pass User Email to Sheets for Apps Script Notification
</commit_message>
<xml_diff>
--- a/backend/plantilla_planificacion_v2.xlsx
+++ b/backend/plantilla_planificacion_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd171dda8de17894/Desktop/cerebro-patio/Cerebro/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_2BB1D69C5B505F711B583E11592FA0B55413FAA7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB8548F3-A11A-4D31-B285-571A22BCE96E}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_2BB1D69C5B505F711B583E11592FA0B55413FAA7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{404E1F99-7BE1-4BD0-AD22-E95B36025010}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,7 +79,7 @@
     <t>Juan Perez</t>
   </si>
   <si>
-    <t>HOLA prueba</t>
+    <t>HOLA prueba2</t>
   </si>
 </sst>
 </file>
@@ -449,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -508,7 +508,7 @@
         <v>46020</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
FEATURE: Add Fuzzy Matching for Technician Names (Fixes Typos)
</commit_message>
<xml_diff>
--- a/backend/plantilla_planificacion_v2.xlsx
+++ b/backend/plantilla_planificacion_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd171dda8de17894/Desktop/cerebro-patio/Cerebro/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="11_2BB1D69C5B505F711B583E11592FA0B55413FAA7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{404E1F99-7BE1-4BD0-AD22-E95B36025010}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="11_2BB1D69C5B505F711B583E11592FA0B55413FAA7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D10579CD-34A4-425D-8BF9-04F33AA07FDF}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -156,10 +156,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -450,12 +446,12 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="5.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.06640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.73046875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.1328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.73046875" bestFit="1" customWidth="1"/>
@@ -508,7 +504,7 @@
         <v>46020</v>
       </c>
       <c r="B2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Fix: Synchronous Email with Rollback for Reliability
</commit_message>
<xml_diff>
--- a/backend/plantilla_planificacion_v2.xlsx
+++ b/backend/plantilla_planificacion_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd171dda8de17894/Desktop/cerebro-patio/Cerebro/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="11_2BB1D69C5B60DD33A738361159DC1037422FF8AD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9566F24B-FDC1-4DF3-9DA3-16CE563BDBFB}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_2BB1D69C5B60DD33A738361159DC1037422FF8AD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD7DC490-F71C-4C4A-8195-FAF28BDF59EF}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>fecha</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>MDVR</t>
+  </si>
+  <si>
+    <t>Soporte</t>
   </si>
 </sst>
 </file>
@@ -470,13 +473,13 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.73046875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.1328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.73046875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.3984375" bestFit="1" customWidth="1"/>
@@ -532,7 +535,7 @@
         <v>46022</v>
       </c>
       <c r="B2">
-        <v>4042512</v>
+        <v>40425123</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -570,13 +573,13 @@
         <v>46022</v>
       </c>
       <c r="B3">
-        <v>4301912</v>
+        <v>43019123</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Fix: Restore Sheet Sync for Consolidated Mode
</commit_message>
<xml_diff>
--- a/backend/plantilla_planificacion_v2.xlsx
+++ b/backend/plantilla_planificacion_v2.xlsx
@@ -10,12 +10,25 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="26" documentId="11_2BB1D69C5B60DD33A738361159DC1037422FF8AD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD7DC490-F71C-4C4A-8195-FAF28BDF59EF}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="2500" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 

</xml_diff>

<commit_message>
Debug: Add verbose score sync endpoint
</commit_message>
<xml_diff>
--- a/backend/plantilla_planificacion_v2.xlsx
+++ b/backend/plantilla_planificacion_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd171dda8de17894/Desktop/cerebro-patio/Cerebro/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_2BB1D69C5B20583D5B582511598680375A87E202" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B13EEBC-16F0-4BFE-9533-6DB89B2154BC}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="11_2BB1D69C5B20583D5B582511598680375A87E202" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B89B3050-1AD5-4A69-8FFE-BB6839A26700}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="2500" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>fecha</t>
   </si>
@@ -82,24 +82,12 @@
     <t>Instalación</t>
   </si>
   <si>
-    <t>GPS, Corta Corriente, Sensor Pta, Sensor Temperatura</t>
-  </si>
-  <si>
-    <t>PANAMERICANA SUR KM. 678 PADRE LAS CASAS</t>
-  </si>
-  <si>
     <t>TEMUCO</t>
   </si>
   <si>
     <t>Región de La Araucanía.</t>
   </si>
   <si>
-    <t>TRPT29</t>
-  </si>
-  <si>
-    <t>DIWATTS</t>
-  </si>
-  <si>
     <t>GPS</t>
   </si>
   <si>
@@ -140,18 +128,6 @@
   </si>
   <si>
     <t>Soporte</t>
-  </si>
-  <si>
-    <t>CAMINO LONGITUDINAL SUR 5201, NOS</t>
-  </si>
-  <si>
-    <t>SAN BERNARDO</t>
-  </si>
-  <si>
-    <t>Región Metropolitana de Santiago.</t>
-  </si>
-  <si>
-    <t>HLPX63</t>
   </si>
   <si>
     <t>CUENTA_CAROZZIDISTRIBUCION</t>
@@ -530,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -619,7 +595,7 @@
         <v>46021</v>
       </c>
       <c r="B2">
-        <v>43572</v>
+        <v>424267</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -628,37 +604,46 @@
         <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
+      <c r="M2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="O2" t="s">
         <v>24</v>
       </c>
-      <c r="K2" t="s">
+      <c r="P2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" t="s">
         <v>25</v>
       </c>
-      <c r="L2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" t="s">
-        <v>29</v>
+      <c r="R2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.45">
@@ -666,131 +651,37 @@
         <v>46021</v>
       </c>
       <c r="B3">
-        <v>42426</v>
+        <v>430947</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="I3" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="J3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="K3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" t="s">
-        <v>36</v>
-      </c>
-      <c r="N3" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" t="s">
-        <v>28</v>
-      </c>
-      <c r="P3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>29</v>
-      </c>
-      <c r="R3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A4" s="2">
-        <v>46021</v>
-      </c>
-      <c r="B4">
-        <v>43567</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" t="s">
-        <v>44</v>
-      </c>
-      <c r="L4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A5" s="2">
-        <v>46021</v>
-      </c>
-      <c r="B5">
-        <v>43094</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" t="s">
         <v>22</v>
-      </c>
-      <c r="H5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5" t="s">
-        <v>46</v>
-      </c>
-      <c r="K5" t="s">
-        <v>44</v>
-      </c>
-      <c r="L5" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: Remove undefined Expense relationship in User model & Add wipe_data utility
</commit_message>
<xml_diff>
--- a/backend/plantilla_planificacion_v2.xlsx
+++ b/backend/plantilla_planificacion_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd171dda8de17894/Desktop/cerebro-patio/Cerebro/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_2BB1D69C5B20583D5B582511598680375A87E202" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B89B3050-1AD5-4A69-8FFE-BB6839A26700}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="11_2BB1D69C5B20583D5B582511598680375A87E202" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{585B8C88-8060-44F2-B54A-65C6B203C801}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="2500" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -509,13 +509,13 @@
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.73046875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.06640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="109.86328125" bestFit="1" customWidth="1"/>
@@ -592,10 +592,10 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B2">
-        <v>424267</v>
+        <v>424267123</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -648,10 +648,10 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B3">
-        <v>430947</v>
+        <v>430947123</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Fix: Allow re-signing a day (Upsert) instead of 400 Error. Ensures points recalculate if tasks are added late.
</commit_message>
<xml_diff>
--- a/backend/plantilla_planificacion_v2.xlsx
+++ b/backend/plantilla_planificacion_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd171dda8de17894/Desktop/cerebro-patio/Cerebro/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_2BB1D69C5B20D7412FD93A11598680375A87E202" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{427E827A-8B48-40C1-91DD-19900E3F7385}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="11_2BB1D69C5B30553B83783511598680375A87E202" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA60B5A4-3680-499C-B02F-78FA8F96ED42}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="2500" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>fecha</t>
   </si>
@@ -94,12 +94,6 @@
     <t>Región de La Araucanía.</t>
   </si>
   <si>
-    <t>TRPT29</t>
-  </si>
-  <si>
-    <t>DIWATTS</t>
-  </si>
-  <si>
     <t>GPS</t>
   </si>
   <si>
@@ -112,61 +106,13 @@
     <t xml:space="preserve"> Sensor Temperatura</t>
   </si>
   <si>
-    <t>GPS, Botón Alámbrico Tablero, Corta Corriente, Sensor Pta, Sensor Pta Adicional, Sensor Temperatura, Sensor Temperatura Adicional</t>
-  </si>
-  <si>
-    <t>RUTA 5 SUR KM 8 SN</t>
-  </si>
-  <si>
-    <t>CHILLAN</t>
-  </si>
-  <si>
-    <t>Región del Ñuble.</t>
-  </si>
-  <si>
-    <t>VE839-POR CONFIRMAR</t>
-  </si>
-  <si>
-    <t>CIAL_ALIMENTOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Botón Alámbrico Tablero</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sensor Pta Adicional</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sensor Temperatura Adicional</t>
-  </si>
-  <si>
-    <t>Soporte</t>
-  </si>
-  <si>
-    <t>CAMINO LONGITUDINAL SUR 5201, NOS</t>
-  </si>
-  <si>
-    <t>SAN BERNARDO</t>
-  </si>
-  <si>
-    <t>Región Metropolitana de Santiago.</t>
-  </si>
-  <si>
-    <t>HLPX63</t>
-  </si>
-  <si>
-    <t>CUENTA_CAROZZIDISTRIBUCION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GUIDO BECK DE RAMBERGA 1884, PADRE DE LAS CASAS </t>
-  </si>
-  <si>
-    <t>BWYY79</t>
-  </si>
-  <si>
-    <t>Pedro Prez</t>
-  </si>
-  <si>
     <t>Pedro Pascal</t>
+  </si>
+  <si>
+    <t>YRPT30</t>
+  </si>
+  <si>
+    <t>HOLA</t>
   </si>
 </sst>
 </file>
@@ -530,15 +476,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="9.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.45">
@@ -599,10 +546,10 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
-        <v>46021</v>
+        <v>46022</v>
       </c>
       <c r="B2">
-        <v>43572</v>
+        <v>3.35723422333344E+16</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -623,157 +570,25 @@
         <v>23</v>
       </c>
       <c r="I2" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" t="s">
         <v>24</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>25</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>26</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>27</v>
-      </c>
-      <c r="N2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A3" s="2">
-        <v>46021</v>
-      </c>
-      <c r="B3">
-        <v>42426</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" t="s">
-        <v>36</v>
-      </c>
-      <c r="N3" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" t="s">
-        <v>28</v>
-      </c>
-      <c r="P3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>29</v>
-      </c>
-      <c r="R3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A4" s="2">
-        <v>46021</v>
-      </c>
-      <c r="B4">
-        <v>43567</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" t="s">
-        <v>44</v>
-      </c>
-      <c r="L4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A5" s="2">
-        <v>46021</v>
-      </c>
-      <c r="B5">
-        <v>43094</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5" t="s">
-        <v>46</v>
-      </c>
-      <c r="K5" t="s">
-        <v>44</v>
-      </c>
-      <c r="L5" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: Smart Signature Status. Return is_signed=False if tasks completed AFTER signature.
</commit_message>
<xml_diff>
--- a/backend/plantilla_planificacion_v2.xlsx
+++ b/backend/plantilla_planificacion_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd171dda8de17894/Desktop/cerebro-patio/Cerebro/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="11_2BB1D69C5B30553B83783511598680375A87E202" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA60B5A4-3680-499C-B02F-78FA8F96ED42}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="11_2BB1D69C5B30553B83783511598680375A87E202" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F4240E9-BAD4-492C-B8D5-22E9B60663BA}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="2500" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -479,7 +479,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -546,10 +546,10 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
-        <v>46022</v>
+        <v>46021</v>
       </c>
       <c r="B2">
-        <v>3.35723422333344E+16</v>
+        <v>123</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Fix: Typos in signatures.py causing SyntaxError (Emergency Fix)
</commit_message>
<xml_diff>
--- a/backend/plantilla_planificacion_v2.xlsx
+++ b/backend/plantilla_planificacion_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd171dda8de17894/Desktop/cerebro-patio/Cerebro/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="11_2BB1D69C5B30553B83783511598680375A87E202" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F4240E9-BAD4-492C-B8D5-22E9B60663BA}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="11_2BB1D69C5B30553B83783511598680375A87E202" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFF8E7BC-2D05-4F55-83C3-82B5C57FECFD}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="2500" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,7 +112,7 @@
     <t>YRPT30</t>
   </si>
   <si>
-    <t>HOLA</t>
+    <t>Brinks</t>
   </si>
 </sst>
 </file>
@@ -479,7 +479,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -549,7 +549,7 @@
         <v>46021</v>
       </c>
       <c r="B2">
-        <v>123</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Fix: Make Signature Status Check robust using Server Time (updated_at) instead of Client Time
</commit_message>
<xml_diff>
--- a/backend/plantilla_planificacion_v2.xlsx
+++ b/backend/plantilla_planificacion_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd171dda8de17894/Desktop/cerebro-patio/Cerebro/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_2BB1D69C5B30553B83783511598680375A87E202" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFF8E7BC-2D05-4F55-83C3-82B5C57FECFD}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="11_2BB1D69C5B30553B83783511598680375A87E202" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3062354B-4D5B-4D82-9C40-3A037E2AFEEF}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="2500" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,7 +112,7 @@
     <t>YRPT30</t>
   </si>
   <si>
-    <t>Brinks</t>
+    <t>Carozzi</t>
   </si>
 </sst>
 </file>
@@ -479,7 +479,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -549,7 +549,7 @@
         <v>46021</v>
       </c>
       <c r="B2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>

</xml_diff>